<commit_message>
Edin article, Login with valid data, tests
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.FunctionalUI.Tests/DataDrivenTests/ArticleData.xlsx
+++ b/Blog-Skeleton/Blog.FunctionalUI.Tests/DataDrivenTests/ArticleData.xlsx
@@ -105,7 +105,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -113,15 +113,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,7 +427,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,69 +439,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>